<commit_message>
Updated with "Sample" example
</commit_message>
<xml_diff>
--- a/selevance/src/test/resources/data/data1.xlsx
+++ b/selevance/src/test/resources/data/data1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Fname</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Upendra Kishore</t>
   </si>
 </sst>
 </file>
@@ -459,9 +462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -498,10 +499,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -512,7 +513,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>

</xml_diff>